<commit_message>
Create Emp Test Case
</commit_message>
<xml_diff>
--- a/TestData/OrangeHRMData.xlsx
+++ b/TestData/OrangeHRMData.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11040" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="User" sheetId="2" r:id="rId2"/>
+    <sheet name="employee" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>EmpName</t>
   </si>
@@ -53,13 +54,34 @@
   </si>
   <si>
     <t>Sai_502</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Navdeep</t>
+  </si>
+  <si>
+    <t>Kaur</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Enabled</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,7 +209,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -222,7 +244,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -399,27 +421,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -427,7 +449,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -442,21 +464,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -470,7 +492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -491,4 +513,53 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>